<commit_message>
Add option to select technical representation of lines (TP or DC-OPF)
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix Auer\Local\Code\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F71739F-3925-4BFB-8F98-97EF8990753A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9CFEE1-D578-4185-A54B-F45E35B893FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-17388" windowWidth="30936" windowHeight="16776" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Network" sheetId="110" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Power Network'!$P$8:$Y$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Power Network'!$Q$8:$Z$19</definedName>
     <definedName name="businfo">#REF!</definedName>
     <definedName name="demand">#REF!</definedName>
     <definedName name="dsmdelaytime">#REF!</definedName>
@@ -32,7 +32,7 @@
     <definedName name="impexp">#REF!</definedName>
     <definedName name="indices">#REF!</definedName>
     <definedName name="inflows">#REF!</definedName>
-    <definedName name="network">'Power Network'!$B$6:$N$20</definedName>
+    <definedName name="network">'Power Network'!$B$6:$O$20</definedName>
     <definedName name="param">#REF!</definedName>
     <definedName name="renewable">#REF!</definedName>
     <definedName name="resprofile">#REF!</definedName>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
   <si>
     <t>[MW]</t>
   </si>
@@ -270,6 +270,18 @@
   </si>
   <si>
     <t>R</t>
+  </si>
+  <si>
+    <t>Technical Representation</t>
+  </si>
+  <si>
+    <t>[DC-OPF, TP]</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>DC-OPF</t>
   </si>
 </sst>
 </file>
@@ -833,11 +845,9 @@
     <tabColor rgb="FF008080"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:Y22"/>
+  <dimension ref="B1:Z22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -846,36 +856,36 @@
     <col min="3" max="3" width="16" style="8" customWidth="1"/>
     <col min="4" max="4" width="8.59765625" style="8" customWidth="1"/>
     <col min="5" max="5" width="13.796875" style="8" customWidth="1"/>
-    <col min="6" max="13" width="13.796875" style="5" customWidth="1"/>
-    <col min="14" max="15" width="16" style="5" customWidth="1"/>
-    <col min="16" max="17" width="14" style="5" customWidth="1"/>
-    <col min="18" max="18" width="15.59765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.796875" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="12.59765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.59765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.3984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="16.59765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="208" width="9.19921875" style="5"/>
-    <col min="209" max="209" width="9.59765625" style="5" customWidth="1"/>
-    <col min="210" max="210" width="1.59765625" style="5" customWidth="1"/>
-    <col min="211" max="211" width="9.19921875" style="5"/>
-    <col min="212" max="212" width="1.59765625" style="5" customWidth="1"/>
-    <col min="213" max="213" width="8.59765625" style="5" customWidth="1"/>
-    <col min="214" max="219" width="9.19921875" style="5"/>
-    <col min="220" max="220" width="1.59765625" style="5" customWidth="1"/>
-    <col min="221" max="224" width="9.19921875" style="5"/>
-    <col min="225" max="225" width="27.59765625" style="5" customWidth="1"/>
-    <col min="226" max="16384" width="9.19921875" style="5"/>
+    <col min="6" max="14" width="13.796875" style="5" customWidth="1"/>
+    <col min="15" max="16" width="16" style="5" customWidth="1"/>
+    <col min="17" max="18" width="14" style="5" customWidth="1"/>
+    <col min="19" max="19" width="15.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.3984375" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="209" width="9.19921875" style="5"/>
+    <col min="210" max="210" width="9.59765625" style="5" customWidth="1"/>
+    <col min="211" max="211" width="1.59765625" style="5" customWidth="1"/>
+    <col min="212" max="212" width="9.19921875" style="5"/>
+    <col min="213" max="213" width="1.59765625" style="5" customWidth="1"/>
+    <col min="214" max="214" width="8.59765625" style="5" customWidth="1"/>
+    <col min="215" max="220" width="9.19921875" style="5"/>
+    <col min="221" max="221" width="1.59765625" style="5" customWidth="1"/>
+    <col min="222" max="225" width="9.19921875" style="5"/>
+    <col min="226" max="226" width="27.59765625" style="5" customWidth="1"/>
+    <col min="227" max="16384" width="9.19921875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:26" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -907,19 +917,22 @@
         <v>12</v>
       </c>
       <c r="N3" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="O3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="P3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:25" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -936,8 +949,9 @@
       <c r="O4" s="6"/>
       <c r="P4" s="6"/>
       <c r="Q4" s="6"/>
-    </row>
-    <row r="5" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -954,8 +968,9 @@
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
       <c r="Q5" s="7"/>
-    </row>
-    <row r="6" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="R5" s="7"/>
+    </row>
+    <row r="6" spans="2:26" x14ac:dyDescent="0.35">
       <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
@@ -984,19 +999,22 @@
         <v>1</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>28</v>
       </c>
       <c r="P6" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="Q6" s="9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="R6" s="9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
@@ -1029,18 +1047,21 @@
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
-      <c r="N7" s="5" t="s">
+      <c r="N7" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O7" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="S7" s="12"/>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
-    </row>
-    <row r="8" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z7" s="12"/>
+    </row>
+    <row r="8" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
@@ -1073,20 +1094,23 @@
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
-      <c r="N8" s="5" t="s">
+      <c r="N8" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="Q8" s="13"/>
       <c r="R8" s="13"/>
-      <c r="S8" s="12"/>
+      <c r="S8" s="13"/>
       <c r="T8" s="12"/>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
       <c r="Y8" s="12"/>
-    </row>
-    <row r="9" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z8" s="12"/>
+    </row>
+    <row r="9" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
@@ -1119,20 +1143,23 @@
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
-      <c r="N9" s="5" t="s">
+      <c r="N9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
-      <c r="S9" s="12"/>
+      <c r="S9" s="3"/>
       <c r="T9" s="12"/>
       <c r="U9" s="12"/>
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
       <c r="X9" s="12"/>
       <c r="Y9" s="12"/>
-    </row>
-    <row r="10" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z9" s="12"/>
+    </row>
+    <row r="10" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
@@ -1165,20 +1192,23 @@
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
-      <c r="N10" s="5" t="s">
+      <c r="N10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O10" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="12"/>
+      <c r="R10" s="8"/>
+      <c r="S10" s="14"/>
       <c r="T10" s="12"/>
       <c r="U10" s="12"/>
       <c r="V10" s="12"/>
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="12"/>
-    </row>
-    <row r="11" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z10" s="12"/>
+    </row>
+    <row r="11" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
@@ -1211,20 +1241,23 @@
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
-      <c r="N11" s="5" t="s">
+      <c r="N11" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O11" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="Q11" s="8"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="12"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="14"/>
       <c r="T11" s="12"/>
       <c r="U11" s="12"/>
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
       <c r="X11" s="12"/>
       <c r="Y11" s="12"/>
-    </row>
-    <row r="12" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z11" s="12"/>
+    </row>
+    <row r="12" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
@@ -1257,20 +1290,23 @@
       </c>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
-      <c r="N12" s="5" t="s">
+      <c r="N12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="12"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="14"/>
       <c r="T12" s="12"/>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="12"/>
-    </row>
-    <row r="13" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z12" s="12"/>
+    </row>
+    <row r="13" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
@@ -1303,20 +1339,23 @@
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O13" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="12"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="14"/>
       <c r="T13" s="12"/>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
       <c r="X13" s="12"/>
       <c r="Y13" s="12"/>
-    </row>
-    <row r="14" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z13" s="12"/>
+    </row>
+    <row r="14" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
@@ -1349,20 +1388,23 @@
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
-      <c r="N14" s="5" t="s">
+      <c r="N14" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="12"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="14"/>
       <c r="T14" s="12"/>
       <c r="U14" s="12"/>
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="12"/>
-    </row>
-    <row r="15" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z14" s="12"/>
+    </row>
+    <row r="15" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B15" s="10" t="s">
         <v>19</v>
       </c>
@@ -1395,20 +1437,23 @@
       </c>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
-      <c r="N15" s="5" t="s">
+      <c r="N15" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O15" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="12"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="14"/>
       <c r="T15" s="12"/>
       <c r="U15" s="12"/>
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="12"/>
-    </row>
-    <row r="16" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z15" s="12"/>
+    </row>
+    <row r="16" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B16" s="10" t="s">
         <v>19</v>
       </c>
@@ -1441,20 +1486,23 @@
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
-      <c r="N16" s="5" t="s">
+      <c r="N16" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O16" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="12"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="14"/>
       <c r="T16" s="12"/>
       <c r="U16" s="12"/>
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
-    </row>
-    <row r="17" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z16" s="12"/>
+    </row>
+    <row r="17" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B17" s="10" t="s">
         <v>20</v>
       </c>
@@ -1487,20 +1535,23 @@
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
-      <c r="N17" s="5" t="s">
+      <c r="N17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O17" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="12"/>
+      <c r="R17" s="8"/>
+      <c r="S17" s="14"/>
       <c r="T17" s="12"/>
       <c r="U17" s="12"/>
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
-    </row>
-    <row r="18" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z17" s="12"/>
+    </row>
+    <row r="18" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B18" s="10" t="s">
         <v>21</v>
       </c>
@@ -1533,20 +1584,23 @@
       </c>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
-      <c r="N18" s="5" t="s">
+      <c r="N18" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="12"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="14"/>
       <c r="T18" s="12"/>
       <c r="U18" s="12"/>
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
       <c r="Y18" s="12"/>
-    </row>
-    <row r="19" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="Z18" s="12"/>
+    </row>
+    <row r="19" spans="2:26" x14ac:dyDescent="0.35">
       <c r="B19" s="10" t="s">
         <v>14</v>
       </c>
@@ -1579,21 +1633,23 @@
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
-      <c r="N19" s="5" t="s">
+      <c r="N19" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="O19" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="12"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="14"/>
       <c r="T19" s="12"/>
       <c r="U19" s="12"/>
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
       <c r="Y19" s="12"/>
-    </row>
-    <row r="20" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="R20" s="14"/>
+      <c r="Z19" s="12"/>
+    </row>
+    <row r="20" spans="2:26" x14ac:dyDescent="0.35">
       <c r="S20" s="14"/>
       <c r="T20" s="14"/>
       <c r="U20" s="14"/>
@@ -1601,10 +1657,10 @@
       <c r="W20" s="14"/>
       <c r="X20" s="14"/>
       <c r="Y20" s="14"/>
-    </row>
-    <row r="21" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="Q21" s="8"/>
-      <c r="R21" s="14"/>
+      <c r="Z20" s="14"/>
+    </row>
+    <row r="21" spans="2:26" x14ac:dyDescent="0.35">
+      <c r="R21" s="8"/>
       <c r="S21" s="14"/>
       <c r="T21" s="14"/>
       <c r="U21" s="14"/>
@@ -1612,9 +1668,9 @@
       <c r="W21" s="14"/>
       <c r="X21" s="14"/>
       <c r="Y21" s="14"/>
-    </row>
-    <row r="22" spans="2:25" x14ac:dyDescent="0.35">
-      <c r="R22" s="14"/>
+      <c r="Z21" s="14"/>
+    </row>
+    <row r="22" spans="2:26" x14ac:dyDescent="0.35">
       <c r="S22" s="14"/>
       <c r="T22" s="14"/>
       <c r="U22" s="14"/>
@@ -1622,6 +1678,7 @@
       <c r="W22" s="14"/>
       <c r="X22" s="14"/>
       <c r="Y22" s="14"/>
+      <c r="Z22" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="15" type="noConversion"/>
@@ -1639,6 +1696,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1784,22 +1856,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1815,28 +1896,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add single-node representation for buses
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Felix Auer\Local\Code\Simplified-Technical-Representation\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF9CFEE1-D578-4185-A54B-F45E35B893FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142DB1A0-25FC-45F3-B867-43A4C39248D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Network" sheetId="110" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
   <si>
     <t>[MW]</t>
   </si>
@@ -275,13 +275,16 @@
     <t>Technical Representation</t>
   </si>
   <si>
-    <t>[DC-OPF, TP]</t>
-  </si>
-  <si>
     <t>TP</t>
   </si>
   <si>
     <t>DC-OPF</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>[DC-OPF, TP, SN]</t>
   </si>
 </sst>
 </file>
@@ -847,45 +850,48 @@
   </sheetPr>
   <dimension ref="B1:Z22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" style="5" customWidth="1"/>
     <col min="2" max="2" width="16" style="5" customWidth="1"/>
     <col min="3" max="3" width="16" style="8" customWidth="1"/>
-    <col min="4" max="4" width="8.59765625" style="8" customWidth="1"/>
-    <col min="5" max="5" width="13.796875" style="8" customWidth="1"/>
-    <col min="6" max="14" width="13.796875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" style="8" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="8" customWidth="1"/>
+    <col min="6" max="13" width="13.85546875" style="5" customWidth="1"/>
+    <col min="14" max="14" width="26.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="15" max="16" width="16" style="5" customWidth="1"/>
     <col min="17" max="18" width="14" style="5" customWidth="1"/>
-    <col min="19" max="19" width="15.59765625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.796875" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" style="5" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.59765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.59765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.3984375" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.59765625" style="5" bestFit="1" customWidth="1"/>
-    <col min="27" max="209" width="9.19921875" style="5"/>
-    <col min="210" max="210" width="9.59765625" style="5" customWidth="1"/>
-    <col min="211" max="211" width="1.59765625" style="5" customWidth="1"/>
-    <col min="212" max="212" width="9.19921875" style="5"/>
-    <col min="213" max="213" width="1.59765625" style="5" customWidth="1"/>
-    <col min="214" max="214" width="8.59765625" style="5" customWidth="1"/>
-    <col min="215" max="220" width="9.19921875" style="5"/>
-    <col min="221" max="221" width="1.59765625" style="5" customWidth="1"/>
-    <col min="222" max="225" width="9.19921875" style="5"/>
-    <col min="226" max="226" width="27.59765625" style="5" customWidth="1"/>
-    <col min="227" max="16384" width="9.19921875" style="5"/>
+    <col min="23" max="23" width="12.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="27" max="209" width="9.140625" style="5"/>
+    <col min="210" max="210" width="9.5703125" style="5" customWidth="1"/>
+    <col min="211" max="211" width="1.5703125" style="5" customWidth="1"/>
+    <col min="212" max="212" width="9.140625" style="5"/>
+    <col min="213" max="213" width="1.5703125" style="5" customWidth="1"/>
+    <col min="214" max="214" width="8.5703125" style="5" customWidth="1"/>
+    <col min="215" max="220" width="9.140625" style="5"/>
+    <col min="221" max="221" width="1.5703125" style="5" customWidth="1"/>
+    <col min="222" max="225" width="9.140625" style="5"/>
+    <col min="226" max="226" width="27.5703125" style="5" customWidth="1"/>
+    <col min="227" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:26" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="15" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -932,7 +938,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -951,7 +957,7 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -970,7 +976,7 @@
       <c r="Q5" s="7"/>
       <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="E6" s="9" t="s">
         <v>5</v>
       </c>
@@ -999,7 +1005,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>28</v>
@@ -1014,7 +1020,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
         <v>14</v>
       </c>
@@ -1043,15 +1049,21 @@
         <v>1</v>
       </c>
       <c r="K7" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>30</v>
+      </c>
+      <c r="P7" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="T7" s="12"/>
       <c r="U7" s="12"/>
@@ -1061,7 +1073,7 @@
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>15</v>
       </c>
@@ -1090,15 +1102,21 @@
         <v>1</v>
       </c>
       <c r="K8" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O8" s="5" t="s">
         <v>31</v>
+      </c>
+      <c r="P8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="R8" s="13"/>
       <c r="S8" s="13"/>
@@ -1110,7 +1128,7 @@
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
         <v>15</v>
       </c>
@@ -1139,15 +1157,21 @@
         <v>1</v>
       </c>
       <c r="K9" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O9" s="5" t="s">
         <v>32</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="R9" s="3"/>
       <c r="S9" s="3"/>
@@ -1159,7 +1183,7 @@
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>16</v>
       </c>
@@ -1188,15 +1212,21 @@
         <v>1</v>
       </c>
       <c r="K10" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O10" s="5" t="s">
         <v>33</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="R10" s="8"/>
       <c r="S10" s="14"/>
@@ -1208,7 +1238,7 @@
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>16</v>
       </c>
@@ -1237,15 +1267,21 @@
         <v>1</v>
       </c>
       <c r="K11" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>34</v>
+      </c>
+      <c r="P11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q11" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="R11" s="8"/>
       <c r="S11" s="14"/>
@@ -1257,7 +1293,7 @@
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>17</v>
       </c>
@@ -1286,15 +1322,21 @@
         <v>1</v>
       </c>
       <c r="K12" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O12" s="5" t="s">
         <v>35</v>
+      </c>
+      <c r="P12" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q12" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="R12" s="8"/>
       <c r="S12" s="14"/>
@@ -1306,7 +1348,7 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
@@ -1335,15 +1377,21 @@
         <v>1</v>
       </c>
       <c r="K13" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O13" s="5" t="s">
         <v>36</v>
+      </c>
+      <c r="P13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q13" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="R13" s="8"/>
       <c r="S13" s="14"/>
@@ -1355,7 +1403,7 @@
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
         <v>17</v>
       </c>
@@ -1384,15 +1432,21 @@
         <v>1</v>
       </c>
       <c r="K14" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O14" s="5" t="s">
         <v>37</v>
+      </c>
+      <c r="P14" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q14" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="R14" s="8"/>
       <c r="S14" s="14"/>
@@ -1404,7 +1458,7 @@
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
         <v>19</v>
       </c>
@@ -1433,15 +1487,21 @@
         <v>1</v>
       </c>
       <c r="K15" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>38</v>
+      </c>
+      <c r="P15" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q15" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="R15" s="8"/>
       <c r="S15" s="14"/>
@@ -1453,7 +1513,7 @@
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
         <v>19</v>
       </c>
@@ -1482,7 +1542,7 @@
         <v>1</v>
       </c>
       <c r="K16" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
@@ -1491,6 +1551,12 @@
       </c>
       <c r="O16" s="5" t="s">
         <v>39</v>
+      </c>
+      <c r="P16" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q16" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="R16" s="8"/>
       <c r="S16" s="14"/>
@@ -1502,7 +1568,7 @@
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
     </row>
-    <row r="17" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
         <v>20</v>
       </c>
@@ -1531,7 +1597,7 @@
         <v>1</v>
       </c>
       <c r="K17" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
@@ -1540,6 +1606,12 @@
       </c>
       <c r="O17" s="5" t="s">
         <v>40</v>
+      </c>
+      <c r="P17" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q17" s="10" t="s">
+        <v>47</v>
       </c>
       <c r="R17" s="8"/>
       <c r="S17" s="14"/>
@@ -1551,7 +1623,7 @@
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
     </row>
-    <row r="18" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
         <v>21</v>
       </c>
@@ -1580,15 +1652,21 @@
         <v>1</v>
       </c>
       <c r="K18" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O18" s="5" t="s">
         <v>41</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q18" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="R18" s="8"/>
       <c r="S18" s="14"/>
@@ -1600,7 +1678,7 @@
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
     </row>
-    <row r="19" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
         <v>14</v>
       </c>
@@ -1629,15 +1707,21 @@
         <v>1</v>
       </c>
       <c r="K19" s="10">
-        <v>800</v>
+        <v>175</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O19" s="5" t="s">
         <v>42</v>
+      </c>
+      <c r="P19" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q19" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="R19" s="8"/>
       <c r="S19" s="14"/>
@@ -1649,7 +1733,7 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row r="20" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:26" x14ac:dyDescent="0.25">
       <c r="S20" s="14"/>
       <c r="T20" s="14"/>
       <c r="U20" s="14"/>
@@ -1659,7 +1743,7 @@
       <c r="Y20" s="14"/>
       <c r="Z20" s="14"/>
     </row>
-    <row r="21" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:26" x14ac:dyDescent="0.25">
       <c r="R21" s="8"/>
       <c r="S21" s="14"/>
       <c r="T21" s="14"/>
@@ -1670,7 +1754,7 @@
       <c r="Y21" s="14"/>
       <c r="Z21" s="14"/>
     </row>
-    <row r="22" spans="2:26" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:26" x14ac:dyDescent="0.25">
       <c r="S22" s="14"/>
       <c r="T22" s="14"/>
       <c r="U22" s="14"/>
@@ -1696,18 +1780,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1857,6 +1941,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1868,14 +1960,6 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Implement merging of SN-connected buses
Update pyomo to 6.8.0
Fix column name in Power_Network (whitespace)
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142DB1A0-25FC-45F3-B867-43A4C39248D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18615A54-AAB0-4043-9920-47C7AEDD3C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Network" sheetId="110" r:id="rId1"/>
@@ -149,9 +149,6 @@
     <t>InService</t>
   </si>
   <si>
-    <t xml:space="preserve">X </t>
-  </si>
-  <si>
     <t>Pmax</t>
   </si>
   <si>
@@ -285,6 +282,9 @@
   </si>
   <si>
     <t>[DC-OPF, TP, SN]</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -850,9 +850,7 @@
   </sheetPr>
   <dimension ref="B1:Z22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -888,7 +886,7 @@
   <sheetData>
     <row r="1" spans="2:26" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="2:26" x14ac:dyDescent="0.25">
@@ -899,43 +897,43 @@
         <v>2</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="N3" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>44</v>
-      </c>
       <c r="O3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="P3" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="Q3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="R3" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="R3" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="4" spans="2:26" x14ac:dyDescent="0.25">
@@ -978,7 +976,7 @@
     </row>
     <row r="6" spans="2:26" x14ac:dyDescent="0.25">
       <c r="E6" s="9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>1</v>
@@ -990,7 +988,7 @@
         <v>1</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J6" s="9" t="s">
         <v>1</v>
@@ -999,36 +997,36 @@
         <v>0</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M6" s="9" t="s">
         <v>1</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="O6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q6" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="R6" s="9" t="s">
         <v>28</v>
-      </c>
-      <c r="Q6" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="9" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B7" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="10">
         <v>1</v>
@@ -1054,18 +1052,19 @@
       <c r="L7" s="10"/>
       <c r="M7" s="10"/>
       <c r="N7" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q7" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="S7" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="T7" s="12"/>
+      <c r="T7" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="U7" s="12"/>
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
@@ -1075,13 +1074,13 @@
     </row>
     <row r="8" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>16</v>
-      </c>
       <c r="D8" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E8" s="10">
         <v>1</v>
@@ -1107,20 +1106,20 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="P8" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="13"/>
+      <c r="S8" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="12"/>
+      <c r="T8" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -1130,13 +1129,13 @@
     </row>
     <row r="9" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B9" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E9" s="10">
         <v>1</v>
@@ -1162,20 +1161,20 @@
       <c r="L9" s="10"/>
       <c r="M9" s="10"/>
       <c r="N9" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>45</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
       <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="12"/>
+      <c r="S9" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="U9" s="12"/>
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
@@ -1185,13 +1184,13 @@
     </row>
     <row r="10" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>17</v>
-      </c>
       <c r="D10" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E10" s="10">
         <v>1</v>
@@ -1217,20 +1216,20 @@
       <c r="L10" s="10"/>
       <c r="M10" s="10"/>
       <c r="N10" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="P10" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q10" s="10" t="s">
-        <v>45</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
       <c r="R10" s="8"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="12"/>
+      <c r="S10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="U10" s="12"/>
       <c r="V10" s="12"/>
       <c r="W10" s="12"/>
@@ -1240,13 +1239,13 @@
     </row>
     <row r="11" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E11" s="10">
         <v>1</v>
@@ -1272,20 +1271,20 @@
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="8"/>
+      <c r="S11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="O11" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="P11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q11" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="R11" s="8"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="12"/>
       <c r="U11" s="12"/>
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
@@ -1295,13 +1294,13 @@
     </row>
     <row r="12" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>18</v>
-      </c>
       <c r="D12" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E12" s="10">
         <v>1</v>
@@ -1327,20 +1326,20 @@
       <c r="L12" s="10"/>
       <c r="M12" s="10"/>
       <c r="N12" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="P12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q12" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="R12" s="8"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="12"/>
+      <c r="T12" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
@@ -1350,13 +1349,13 @@
     </row>
     <row r="13" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E13" s="10">
         <v>1</v>
@@ -1382,20 +1381,20 @@
       <c r="L13" s="10"/>
       <c r="M13" s="10"/>
       <c r="N13" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="P13" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q13" s="10" t="s">
-        <v>45</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
       <c r="R13" s="8"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="12"/>
+      <c r="S13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T13" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
@@ -1405,13 +1404,13 @@
     </row>
     <row r="14" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E14" s="10">
         <v>1</v>
@@ -1437,20 +1436,20 @@
       <c r="L14" s="10"/>
       <c r="M14" s="10"/>
       <c r="N14" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="P14" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q14" s="10" t="s">
-        <v>45</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
       <c r="R14" s="8"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="12"/>
+      <c r="S14" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="U14" s="12"/>
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
@@ -1460,13 +1459,13 @@
     </row>
     <row r="15" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="10" t="s">
-        <v>20</v>
-      </c>
       <c r="D15" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E15" s="10">
         <v>1</v>
@@ -1492,20 +1491,20 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="O15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T15" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="O15" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="P15" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q15" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="R15" s="8"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="12"/>
       <c r="U15" s="12"/>
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
@@ -1515,13 +1514,13 @@
     </row>
     <row r="16" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B16" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E16" s="10">
         <v>1</v>
@@ -1547,20 +1546,20 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="P16" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q16" s="10" t="s">
-        <v>47</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
       <c r="R16" s="8"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="12"/>
+      <c r="S16" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="T16" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="U16" s="12"/>
       <c r="V16" s="12"/>
       <c r="W16" s="12"/>
@@ -1570,13 +1569,13 @@
     </row>
     <row r="17" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="10" t="s">
-        <v>21</v>
-      </c>
       <c r="D17" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E17" s="10">
         <v>1</v>
@@ -1602,20 +1601,20 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="P17" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q17" s="10" t="s">
-        <v>47</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10"/>
       <c r="R17" s="8"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="12"/>
+      <c r="S17" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="T17" s="5" t="s">
+        <v>46</v>
+      </c>
       <c r="U17" s="12"/>
       <c r="V17" s="12"/>
       <c r="W17" s="12"/>
@@ -1625,13 +1624,13 @@
     </row>
     <row r="18" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>22</v>
-      </c>
       <c r="D18" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E18" s="10">
         <v>1</v>
@@ -1657,20 +1656,20 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="P18" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q18" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10"/>
+      <c r="R18" s="8"/>
+      <c r="S18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="R18" s="8"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="12"/>
+      <c r="T18" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="U18" s="12"/>
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
@@ -1680,13 +1679,13 @@
     </row>
     <row r="19" spans="2:26" x14ac:dyDescent="0.25">
       <c r="B19" s="10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" s="10">
         <v>1</v>
@@ -1712,20 +1711,20 @@
       <c r="L19" s="10"/>
       <c r="M19" s="10"/>
       <c r="N19" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="P19" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="Q19" s="10" t="s">
-        <v>45</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10"/>
       <c r="R19" s="8"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="12"/>
+      <c r="S19" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="T19" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="U19" s="12"/>
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
@@ -1780,18 +1779,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1941,14 +1940,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -1960,6 +1951,14 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix updating of hGenerator_to_Buses (after SN-merge)
Update assert message
Update Power_Network.xlsx to remove superfluous columns
Adjust tested case studies
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18615A54-AAB0-4043-9920-47C7AEDD3C0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B8C4A1-4D27-48AC-B22F-20FFB3E72CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Network" sheetId="110" r:id="rId1"/>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
   <si>
     <t>[MW]</t>
   </si>
@@ -850,7 +850,9 @@
   </sheetPr>
   <dimension ref="B1:Z22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1059,12 +1061,6 @@
       </c>
       <c r="P7" s="10"/>
       <c r="Q7" s="10"/>
-      <c r="S7" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T7" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="U7" s="12"/>
       <c r="V7" s="12"/>
       <c r="W7" s="12"/>
@@ -1114,12 +1110,6 @@
       <c r="P8" s="10"/>
       <c r="Q8" s="10"/>
       <c r="R8" s="13"/>
-      <c r="S8" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="U8" s="12"/>
       <c r="V8" s="12"/>
       <c r="W8" s="12"/>
@@ -1169,12 +1159,6 @@
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="3"/>
-      <c r="S9" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T9" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="U9" s="12"/>
       <c r="V9" s="12"/>
       <c r="W9" s="12"/>
@@ -1224,12 +1208,6 @@
       <c r="P10" s="10"/>
       <c r="Q10" s="10"/>
       <c r="R10" s="8"/>
-      <c r="S10" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="U10" s="12"/>
       <c r="V10" s="12"/>
       <c r="W10" s="12"/>
@@ -1271,7 +1249,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>33</v>
@@ -1279,12 +1257,6 @@
       <c r="P11" s="10"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="8"/>
-      <c r="S11" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="U11" s="12"/>
       <c r="V11" s="12"/>
       <c r="W11" s="12"/>
@@ -1334,12 +1306,6 @@
       <c r="P12" s="10"/>
       <c r="Q12" s="10"/>
       <c r="R12" s="8"/>
-      <c r="S12" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="U12" s="12"/>
       <c r="V12" s="12"/>
       <c r="W12" s="12"/>
@@ -1389,12 +1355,6 @@
       <c r="P13" s="10"/>
       <c r="Q13" s="10"/>
       <c r="R13" s="8"/>
-      <c r="S13" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T13" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="U13" s="12"/>
       <c r="V13" s="12"/>
       <c r="W13" s="12"/>
@@ -1444,12 +1404,6 @@
       <c r="P14" s="10"/>
       <c r="Q14" s="10"/>
       <c r="R14" s="8"/>
-      <c r="S14" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T14" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="U14" s="12"/>
       <c r="V14" s="12"/>
       <c r="W14" s="12"/>
@@ -1499,12 +1453,6 @@
       <c r="P15" s="10"/>
       <c r="Q15" s="10"/>
       <c r="R15" s="8"/>
-      <c r="S15" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T15" s="5" t="s">
-        <v>46</v>
-      </c>
       <c r="U15" s="12"/>
       <c r="V15" s="12"/>
       <c r="W15" s="12"/>
@@ -1554,14 +1502,7 @@
       <c r="P16" s="10"/>
       <c r="Q16" s="10"/>
       <c r="R16" s="8"/>
-      <c r="S16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="T16" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="U16" s="12"/>
-      <c r="V16" s="12"/>
+      <c r="V16" s="8"/>
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
       <c r="Y16" s="12"/>
@@ -1609,14 +1550,7 @@
       <c r="P17" s="10"/>
       <c r="Q17" s="10"/>
       <c r="R17" s="8"/>
-      <c r="S17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="T17" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="U17" s="12"/>
-      <c r="V17" s="12"/>
+      <c r="V17" s="8"/>
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
       <c r="Y17" s="12"/>
@@ -1664,12 +1598,6 @@
       <c r="P18" s="10"/>
       <c r="Q18" s="10"/>
       <c r="R18" s="8"/>
-      <c r="S18" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T18" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="U18" s="12"/>
       <c r="V18" s="12"/>
       <c r="W18" s="12"/>
@@ -1719,12 +1647,6 @@
       <c r="P19" s="10"/>
       <c r="Q19" s="10"/>
       <c r="R19" s="8"/>
-      <c r="S19" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="T19" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="U19" s="12"/>
       <c r="V19" s="12"/>
       <c r="W19" s="12"/>
@@ -1785,15 +1707,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1939,6 +1852,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
@@ -1956,14 +1878,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1979,4 +1893,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust pReactance to match eDC_ExiLinePij (incl. variable names)
Adjust Power_Network to have candidate lines
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21B8C4A1-4D27-48AC-B22F-20FFB3E72CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDC4EAD-0368-4A32-A72C-55495A117A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="17550" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Network" sheetId="110" r:id="rId1"/>
@@ -851,7 +851,7 @@
   <dimension ref="B1:Z22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1471,7 +1471,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="11">
         <v>5.0000000000000001E-3</v>
@@ -1519,7 +1519,7 @@
         <v>5</v>
       </c>
       <c r="E17" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F17" s="11">
         <v>7.0000000000000001E-3</v>
@@ -1567,7 +1567,7 @@
         <v>5</v>
       </c>
       <c r="E18" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F18" s="11">
         <v>6.0000000000000001E-3</v>
@@ -1636,7 +1636,9 @@
       <c r="K19" s="10">
         <v>175</v>
       </c>
-      <c r="L19" s="10"/>
+      <c r="L19" s="10">
+        <v>100</v>
+      </c>
       <c r="M19" s="10"/>
       <c r="N19" s="10" t="s">
         <v>44</v>
@@ -1701,9 +1703,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1853,26 +1858,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1896,9 +1890,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust data-files of example to also test expansion planning
Set one enableInvest = 1 for Power_VRES
Set two enableInvest = 1 for Power_Storage
Add investment candidate for Power_Network
Set pEnablePowerImportExport = No
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDC4EAD-0368-4A32-A72C-55495A117A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5958C3-2E4D-4336-8B41-50EED46A489A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-135" yWindow="-135" windowWidth="29070" windowHeight="17550" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Power Network" sheetId="110" r:id="rId1"/>
@@ -851,7 +851,7 @@
   <dimension ref="B1:Z22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1051,7 +1051,9 @@
       <c r="K7" s="10">
         <v>175</v>
       </c>
-      <c r="L7" s="10"/>
+      <c r="L7" s="10">
+        <v>10</v>
+      </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10" t="s">
         <v>45</v>
@@ -1295,7 +1297,9 @@
       <c r="K12" s="10">
         <v>175</v>
       </c>
-      <c r="L12" s="10"/>
+      <c r="L12" s="10">
+        <v>50</v>
+      </c>
       <c r="M12" s="10"/>
       <c r="N12" s="10" t="s">
         <v>45</v>
@@ -1393,7 +1397,9 @@
       <c r="K14" s="10">
         <v>175</v>
       </c>
-      <c r="L14" s="10"/>
+      <c r="L14" s="10">
+        <v>30</v>
+      </c>
       <c r="M14" s="10"/>
       <c r="N14" s="10" t="s">
         <v>44</v>
@@ -1712,6 +1718,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1857,12 +1869,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
@@ -1872,6 +1878,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1887,20 +1909,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust Power_Network to have FxChargeRate filled out, adjust pFixedCost
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\Simplified-Technical-Representation\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F5958C3-2E4D-4336-8B41-50EED46A489A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5E3D5A-7035-476C-87B6-5964B8893F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -850,9 +850,7 @@
   </sheetPr>
   <dimension ref="B1:Z22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1054,7 +1052,9 @@
       <c r="L7" s="10">
         <v>10</v>
       </c>
-      <c r="M7" s="10"/>
+      <c r="M7" s="10">
+        <v>1</v>
+      </c>
       <c r="N7" s="10" t="s">
         <v>45</v>
       </c>
@@ -1300,7 +1300,9 @@
       <c r="L12" s="10">
         <v>50</v>
       </c>
-      <c r="M12" s="10"/>
+      <c r="M12" s="10">
+        <v>2</v>
+      </c>
       <c r="N12" s="10" t="s">
         <v>45</v>
       </c>
@@ -1377,7 +1379,7 @@
         <v>5</v>
       </c>
       <c r="E14" s="10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="11">
         <v>1E-3</v>
@@ -1400,7 +1402,9 @@
       <c r="L14" s="10">
         <v>30</v>
       </c>
-      <c r="M14" s="10"/>
+      <c r="M14" s="10">
+        <v>3</v>
+      </c>
       <c r="N14" s="10" t="s">
         <v>44</v>
       </c>
@@ -1645,7 +1649,9 @@
       <c r="L19" s="10">
         <v>100</v>
       </c>
-      <c r="M19" s="10"/>
+      <c r="M19" s="10">
+        <v>0.5</v>
+      </c>
       <c r="N19" s="10" t="s">
         <v>44</v>
       </c>
@@ -1709,21 +1715,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1869,10 +1860,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1894,19 +1910,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add LEGO.py as standard way of executing LEGO
Switch Power_Network for example to have DC-OPF for all lines
Update Conda-Activation-Scripts
Add rich-argparse to environment.yml
Add .gitattributes to fix potential line-ending issues
Commit line-ending changes
Sanitize caseStudyFolder (if it doesn't end with '/')
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC5E3D5A-7035-476C-87B6-5964B8893F1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B184806D-4747-49A7-A2B0-3EBCB06919D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -138,7 +138,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="47">
   <si>
     <t>[MW]</t>
   </si>
@@ -272,13 +272,7 @@
     <t>Technical Representation</t>
   </si>
   <si>
-    <t>TP</t>
-  </si>
-  <si>
     <t>DC-OPF</t>
-  </si>
-  <si>
-    <t>SN</t>
   </si>
   <si>
     <t>[DC-OPF, TP, SN]</t>
@@ -900,7 +894,7 @@
         <v>42</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H3" s="4" t="s">
         <v>6</v>
@@ -1003,7 +997,7 @@
         <v>1</v>
       </c>
       <c r="N6" s="9" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O6" s="9" t="s">
         <v>27</v>
@@ -1056,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O7" s="5" t="s">
         <v>29</v>
@@ -1104,7 +1098,7 @@
       <c r="L8" s="10"/>
       <c r="M8" s="10"/>
       <c r="N8" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O8" s="5" t="s">
         <v>30</v>
@@ -1251,7 +1245,7 @@
       <c r="L11" s="10"/>
       <c r="M11" s="10"/>
       <c r="N11" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O11" s="5" t="s">
         <v>33</v>
@@ -1304,7 +1298,7 @@
         <v>2</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O12" s="5" t="s">
         <v>34</v>
@@ -1455,7 +1449,7 @@
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O15" s="5" t="s">
         <v>37</v>
@@ -1504,7 +1498,7 @@
       <c r="L16" s="10"/>
       <c r="M16" s="10"/>
       <c r="N16" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O16" s="5" t="s">
         <v>38</v>
@@ -1552,7 +1546,7 @@
       <c r="L17" s="10"/>
       <c r="M17" s="10"/>
       <c r="N17" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O17" s="5" t="s">
         <v>39</v>
@@ -1600,7 +1594,7 @@
       <c r="L18" s="10"/>
       <c r="M18" s="10"/>
       <c r="N18" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O18" s="5" t="s">
         <v>40</v>
@@ -1715,6 +1709,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -1860,35 +1869,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1910,9 +1894,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Adjust Power_Network to v0.0.4r
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FelixAuer\Git\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D158E5-90D6-49E0-BCA1-FF749010342A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C97D547-6BC3-46E0-9E86-C774A2CC0577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32565" yWindow="-21720" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="89">
   <si>
     <t>[MW]</t>
   </si>
@@ -249,12 +249,6 @@
     <t>i</t>
   </si>
   <si>
-    <t>comYear</t>
-  </si>
-  <si>
-    <t>decomYear</t>
-  </si>
-  <si>
     <t>dataPackage</t>
   </si>
   <si>
@@ -408,9 +402,6 @@
     <t>Year where it is de-commissioned (31.12.xxxx)</t>
   </si>
   <si>
-    <t>v0.0.3</t>
-  </si>
-  <si>
     <t>[0, 1]</t>
   </si>
   <si>
@@ -421,6 +412,18 @@
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>v0.0.4r</t>
+  </si>
+  <si>
+    <t>excl</t>
+  </si>
+  <si>
+    <t>YearCom</t>
+  </si>
+  <si>
+    <t>YearDecom</t>
   </si>
 </sst>
 </file>
@@ -1077,26 +1080,26 @@
         <v>22</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>17</v>
@@ -1108,22 +1111,22 @@
         <v>3</v>
       </c>
       <c r="I3" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="N3" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>18</v>
@@ -1143,7 +1146,7 @@
     </row>
     <row r="4" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>28</v>
@@ -1152,181 +1155,181 @@
         <v>29</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F4" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="I4" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I4" s="13" t="s">
-        <v>60</v>
-      </c>
       <c r="J4" s="13" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K4" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O4" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="L4" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>66</v>
-      </c>
       <c r="P4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="R4" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="Q4" s="13" t="s">
+      <c r="S4" s="13" t="s">
         <v>31</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" s="15" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G5" s="15" t="s">
+      <c r="H5" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>59</v>
-      </c>
       <c r="I5" s="15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="J5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="L5" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="L5" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>67</v>
-      </c>
       <c r="P5" s="15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q5" s="15" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="R5" s="15" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="S5" s="15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:22" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="H6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="I6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>38</v>
-      </c>
       <c r="M6" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="N6" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="P6" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="R6" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>1</v>
@@ -1347,7 +1350,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>5</v>
@@ -1365,10 +1368,10 @@
         <v>16</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1381,7 +1384,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F8" s="22">
         <v>2E-3</v>
@@ -1418,10 +1421,10 @@
         <v>2029</v>
       </c>
       <c r="R8" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S8" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
@@ -1437,7 +1440,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F9" s="22">
         <v>4.0000000000000001E-3</v>
@@ -1472,10 +1475,10 @@
         <v>2029</v>
       </c>
       <c r="R9" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S9" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
@@ -1491,7 +1494,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F10" s="22">
         <v>6.0000000000000001E-3</v>
@@ -1526,10 +1529,10 @@
         <v>2029</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S10" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
@@ -1545,7 +1548,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F11" s="22">
         <v>8.0000000000000002E-3</v>
@@ -1580,10 +1583,10 @@
         <v>2029</v>
       </c>
       <c r="R11" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S11" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
@@ -1599,7 +1602,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F12" s="22">
         <v>7.0000000000000001E-3</v>
@@ -1634,10 +1637,10 @@
         <v>2050</v>
       </c>
       <c r="R12" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S12" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
@@ -1653,7 +1656,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F13" s="22">
         <v>5.0000000000000001E-3</v>
@@ -1690,10 +1693,10 @@
         <v>2050</v>
       </c>
       <c r="R13" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S13" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
@@ -1709,7 +1712,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F14" s="22">
         <v>3.0000000000000001E-3</v>
@@ -1744,10 +1747,10 @@
         <v>2050</v>
       </c>
       <c r="R14" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S14" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
@@ -1755,7 +1758,7 @@
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="21" t="s">
@@ -1765,7 +1768,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F15" s="22">
         <v>1E-3</v>
@@ -1802,10 +1805,10 @@
         <v>2050</v>
       </c>
       <c r="R15" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S15" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
@@ -1821,7 +1824,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F16" s="22">
         <v>3.0000000000000001E-3</v>
@@ -1856,10 +1859,10 @@
         <v>2050</v>
       </c>
       <c r="R16" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S16" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
@@ -1867,7 +1870,7 @@
     </row>
     <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="21" t="s">
@@ -1877,7 +1880,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F17" s="22">
         <v>5.0000000000000001E-3</v>
@@ -1912,10 +1915,10 @@
         <v>2050</v>
       </c>
       <c r="R17" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S17" s="19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
@@ -1923,7 +1926,7 @@
     </row>
     <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="21" t="s">
@@ -1933,7 +1936,7 @@
         <v>13</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F18" s="22">
         <v>7.0000000000000001E-3</v>
@@ -1968,10 +1971,10 @@
         <v>2050</v>
       </c>
       <c r="R18" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S18" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
@@ -1979,7 +1982,7 @@
     </row>
     <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="21" t="s">
@@ -1989,7 +1992,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F19" s="22">
         <v>6.0000000000000001E-3</v>
@@ -2024,10 +2027,10 @@
         <v>2050</v>
       </c>
       <c r="R19" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S19" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:22" x14ac:dyDescent="0.25">
@@ -2040,7 +2043,7 @@
         <v>9</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F20" s="22">
         <v>6.0000000000000001E-3</v>
@@ -2077,10 +2080,10 @@
         <v>2050</v>
       </c>
       <c r="R20" s="19" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="S20" s="26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2093,6 +2096,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2238,15 +2250,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2254,6 +2257,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2267,14 +2278,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Error correction (part 1 of 1000000)
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin Walenta\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1262AABA-710B-4BD2-8A85-294B842D7838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A756A1-3040-444B-9EB9-FC51E6791626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5110" yWindow="2290" windowWidth="28800" windowHeight="15430" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="110" r:id="rId1"/>
@@ -216,9 +216,6 @@
     <t>Technical Representation</t>
   </si>
   <si>
-    <t>DC-OPF</t>
-  </si>
-  <si>
     <t>[DC-OPF, TP, SN]</t>
   </si>
   <si>
@@ -424,6 +421,9 @@
   </si>
   <si>
     <t>YearDecom</t>
+  </si>
+  <si>
+    <t>SOCP</t>
   </si>
 </sst>
 </file>
@@ -435,7 +435,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -531,6 +531,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color rgb="FFCE9178"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="11">
@@ -630,7 +636,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -699,6 +705,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1036,300 +1045,300 @@
       <selection activeCell="R6" sqref="R6:S6"/>
       <selection pane="topRight" activeCell="R6" sqref="R6:S6"/>
       <selection pane="bottomLeft" activeCell="R6" sqref="R6:S6"/>
-      <selection pane="bottomRight" activeCell="N31" sqref="N31"/>
+      <selection pane="bottomRight" activeCell="O8" sqref="O8:O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.8984375" style="3" customWidth="1"/>
     <col min="2" max="2" width="15" style="3" customWidth="1"/>
-    <col min="3" max="5" width="14.5703125" style="4" customWidth="1"/>
-    <col min="6" max="11" width="12.85546875" style="3" customWidth="1"/>
+    <col min="3" max="5" width="14.59765625" style="4" customWidth="1"/>
+    <col min="6" max="11" width="12.8984375" style="3" customWidth="1"/>
     <col min="12" max="13" width="15" style="3" customWidth="1"/>
-    <col min="14" max="14" width="28.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="28.8984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.296875" style="3" customWidth="1"/>
     <col min="16" max="17" width="21" style="3" customWidth="1"/>
-    <col min="18" max="19" width="25.85546875" style="3" customWidth="1"/>
+    <col min="18" max="19" width="25.8984375" style="3" customWidth="1"/>
     <col min="20" max="20" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.8984375" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="209" width="9.140625" style="3"/>
-    <col min="210" max="210" width="9.5703125" style="3" customWidth="1"/>
-    <col min="211" max="211" width="1.5703125" style="3" customWidth="1"/>
-    <col min="212" max="212" width="9.140625" style="3"/>
-    <col min="213" max="213" width="1.5703125" style="3" customWidth="1"/>
-    <col min="214" max="214" width="8.5703125" style="3" customWidth="1"/>
-    <col min="215" max="220" width="9.140625" style="3"/>
-    <col min="221" max="221" width="1.5703125" style="3" customWidth="1"/>
-    <col min="222" max="225" width="9.140625" style="3"/>
-    <col min="226" max="226" width="27.5703125" style="3" customWidth="1"/>
-    <col min="227" max="16384" width="9.140625" style="3"/>
+    <col min="23" max="23" width="12.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="209" width="9.09765625" style="3"/>
+    <col min="210" max="210" width="9.59765625" style="3" customWidth="1"/>
+    <col min="211" max="211" width="1.59765625" style="3" customWidth="1"/>
+    <col min="212" max="212" width="9.09765625" style="3"/>
+    <col min="213" max="213" width="1.59765625" style="3" customWidth="1"/>
+    <col min="214" max="214" width="8.59765625" style="3" customWidth="1"/>
+    <col min="215" max="220" width="9.09765625" style="3"/>
+    <col min="221" max="221" width="1.59765625" style="3" customWidth="1"/>
+    <col min="222" max="225" width="9.09765625" style="3"/>
+    <col min="226" max="226" width="27.59765625" style="3" customWidth="1"/>
+    <col min="227" max="16384" width="9.09765625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
       <c r="B2" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B3" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="11" t="s">
-        <v>42</v>
-      </c>
       <c r="E3" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="G3" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>3</v>
       </c>
       <c r="I3" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="J3" s="11" t="s">
         <v>50</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>2</v>
       </c>
       <c r="L3" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N3" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="N3" s="11" t="s">
-        <v>67</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>18</v>
       </c>
       <c r="P3" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Q3" s="11" t="s">
+      <c r="R3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="R3" s="11" t="s">
+      <c r="S3" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="S3" s="11" t="s">
+    </row>
+    <row r="4" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" s="13" t="s">
         <v>27</v>
       </c>
+      <c r="C4" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="P4" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q4" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="R4" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="S4" s="13" t="s">
+        <v>30</v>
+      </c>
     </row>
-    <row r="4" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E4" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G4" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="H4" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="L4" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="N4" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="O4" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="Q4" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="S4" s="13" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:22" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="17"/>
       <c r="B5" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="K5" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="M5" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="N5" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="P5" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q5" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="R5" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="S5" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F5" s="15" t="s">
-        <v>53</v>
-      </c>
-      <c r="G5" s="15" t="s">
-        <v>55</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="J5" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="L5" s="15" t="s">
-        <v>82</v>
-      </c>
-      <c r="M5" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="N5" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="P5" s="15" t="s">
-        <v>79</v>
-      </c>
-      <c r="Q5" s="15" t="s">
-        <v>80</v>
-      </c>
-      <c r="R5" s="15" t="s">
-        <v>78</v>
-      </c>
-      <c r="S5" s="15" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="6" spans="1:22" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
       <c r="A6" s="17"/>
       <c r="B6" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="D6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="M6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="N6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="O6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="P6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="Q6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="R6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="J6" s="16" t="s">
+      <c r="S6" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="M6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="N6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="O6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="R6" s="16" t="s">
-        <v>36</v>
-      </c>
-      <c r="S6" s="16" t="s">
-        <v>36</v>
-      </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>38</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>1</v>
@@ -1350,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M7" s="5" t="s">
         <v>5</v>
@@ -1359,7 +1368,7 @@
         <v>5</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P7" s="5" t="s">
         <v>16</v>
@@ -1368,13 +1377,13 @@
         <v>16</v>
       </c>
       <c r="R7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S7" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="S7" s="5" t="s">
-        <v>40</v>
-      </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A8" s="24"/>
       <c r="B8" s="20"/>
       <c r="C8" s="21" t="s">
@@ -1384,7 +1393,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F8" s="22">
         <v>2E-3</v>
@@ -1411,8 +1420,8 @@
       <c r="N8" s="25">
         <v>10</v>
       </c>
-      <c r="O8" s="19" t="s">
-        <v>19</v>
+      <c r="O8" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P8" s="19">
         <v>1980</v>
@@ -1421,16 +1430,16 @@
         <v>2029</v>
       </c>
       <c r="R8" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S8" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="S8" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="T8" s="6"/>
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A9" s="24"/>
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
@@ -1440,7 +1449,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F9" s="22">
         <v>4.0000000000000001E-3</v>
@@ -1465,8 +1474,8 @@
       </c>
       <c r="M9" s="25"/>
       <c r="N9" s="25"/>
-      <c r="O9" s="19" t="s">
-        <v>19</v>
+      <c r="O9" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P9" s="19">
         <v>1980</v>
@@ -1475,16 +1484,16 @@
         <v>2029</v>
       </c>
       <c r="R9" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S9" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="S9" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="T9" s="6"/>
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A10" s="24"/>
       <c r="B10" s="20"/>
       <c r="C10" s="21" t="s">
@@ -1494,7 +1503,7 @@
         <v>11</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10" s="22">
         <v>6.0000000000000001E-3</v>
@@ -1519,8 +1528,8 @@
       </c>
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
-      <c r="O10" s="19" t="s">
-        <v>19</v>
+      <c r="O10" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P10" s="19">
         <v>1980</v>
@@ -1529,16 +1538,16 @@
         <v>2029</v>
       </c>
       <c r="R10" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S10" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="S10" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="T10" s="6"/>
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A11" s="24"/>
       <c r="B11" s="20"/>
       <c r="C11" s="21" t="s">
@@ -1548,7 +1557,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="22">
         <v>8.0000000000000002E-3</v>
@@ -1573,8 +1582,8 @@
       </c>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
-      <c r="O11" s="19" t="s">
-        <v>19</v>
+      <c r="O11" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P11" s="19">
         <v>1980</v>
@@ -1583,16 +1592,16 @@
         <v>2029</v>
       </c>
       <c r="R11" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S11" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="S11" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="T11" s="6"/>
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A12" s="24"/>
       <c r="B12" s="20"/>
       <c r="C12" s="21" t="s">
@@ -1602,7 +1611,7 @@
         <v>11</v>
       </c>
       <c r="E12" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="22">
         <v>7.0000000000000001E-3</v>
@@ -1627,8 +1636,8 @@
       </c>
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
-      <c r="O12" s="19" t="s">
-        <v>19</v>
+      <c r="O12" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P12" s="19">
         <v>1980</v>
@@ -1637,16 +1646,16 @@
         <v>2050</v>
       </c>
       <c r="R12" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S12" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="S12" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A13" s="24"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21" t="s">
@@ -1656,7 +1665,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F13" s="22">
         <v>5.0000000000000001E-3</v>
@@ -1683,8 +1692,8 @@
       <c r="N13" s="25">
         <v>100</v>
       </c>
-      <c r="O13" s="19" t="s">
-        <v>19</v>
+      <c r="O13" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P13" s="19">
         <v>1980</v>
@@ -1693,16 +1702,16 @@
         <v>2050</v>
       </c>
       <c r="R13" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S13" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="S13" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="T13" s="6"/>
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A14" s="24"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21" t="s">
@@ -1712,7 +1721,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F14" s="22">
         <v>3.0000000000000001E-3</v>
@@ -1737,8 +1746,8 @@
       </c>
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
-      <c r="O14" s="19" t="s">
-        <v>19</v>
+      <c r="O14" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P14" s="19">
         <v>1980</v>
@@ -1747,18 +1756,18 @@
         <v>2050</v>
       </c>
       <c r="R14" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S14" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="S14" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A15" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="21" t="s">
@@ -1768,7 +1777,7 @@
         <v>14</v>
       </c>
       <c r="E15" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15" s="22">
         <v>1E-3</v>
@@ -1795,8 +1804,8 @@
       <c r="N15" s="25">
         <v>90</v>
       </c>
-      <c r="O15" s="19" t="s">
-        <v>19</v>
+      <c r="O15" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P15" s="19">
         <v>1980</v>
@@ -1805,16 +1814,16 @@
         <v>2050</v>
       </c>
       <c r="R15" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S15" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="S15" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A16" s="24"/>
       <c r="B16" s="20"/>
       <c r="C16" s="21" t="s">
@@ -1824,7 +1833,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F16" s="22">
         <v>3.0000000000000001E-3</v>
@@ -1849,8 +1858,8 @@
       </c>
       <c r="M16" s="25"/>
       <c r="N16" s="25"/>
-      <c r="O16" s="19" t="s">
-        <v>19</v>
+      <c r="O16" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P16" s="19">
         <v>1980</v>
@@ -1859,18 +1868,18 @@
         <v>2050</v>
       </c>
       <c r="R16" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S16" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="S16" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="T16" s="7"/>
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B17" s="20"/>
       <c r="C17" s="21" t="s">
@@ -1880,7 +1889,7 @@
         <v>13</v>
       </c>
       <c r="E17" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F17" s="22">
         <v>5.0000000000000001E-3</v>
@@ -1905,8 +1914,8 @@
       </c>
       <c r="M17" s="25"/>
       <c r="N17" s="25"/>
-      <c r="O17" s="19" t="s">
-        <v>19</v>
+      <c r="O17" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P17" s="19">
         <v>1980</v>
@@ -1915,18 +1924,18 @@
         <v>2050</v>
       </c>
       <c r="R17" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="S17" s="19" t="s">
         <v>72</v>
-      </c>
-      <c r="S17" s="19" t="s">
-        <v>73</v>
       </c>
       <c r="T17" s="7"/>
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="21" t="s">
@@ -1936,7 +1945,7 @@
         <v>13</v>
       </c>
       <c r="E18" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F18" s="22">
         <v>7.0000000000000001E-3</v>
@@ -1961,8 +1970,8 @@
       </c>
       <c r="M18" s="25"/>
       <c r="N18" s="25"/>
-      <c r="O18" s="19" t="s">
-        <v>19</v>
+      <c r="O18" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P18" s="19">
         <v>2030</v>
@@ -1971,18 +1980,18 @@
         <v>2050</v>
       </c>
       <c r="R18" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S18" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="T18" s="7"/>
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" s="24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B19" s="20"/>
       <c r="C19" s="21" t="s">
@@ -1992,7 +2001,7 @@
         <v>14</v>
       </c>
       <c r="E19" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F19" s="22">
         <v>6.0000000000000001E-3</v>
@@ -2017,8 +2026,8 @@
       </c>
       <c r="M19" s="25"/>
       <c r="N19" s="25"/>
-      <c r="O19" s="19" t="s">
-        <v>19</v>
+      <c r="O19" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P19" s="19">
         <v>2030</v>
@@ -2027,13 +2036,13 @@
         <v>2050</v>
       </c>
       <c r="R19" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S19" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A20" s="24"/>
       <c r="B20" s="20"/>
       <c r="C20" s="21" t="s">
@@ -2043,7 +2052,7 @@
         <v>9</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F20" s="22">
         <v>6.0000000000000001E-3</v>
@@ -2070,8 +2079,8 @@
       <c r="N20" s="25">
         <v>50</v>
       </c>
-      <c r="O20" s="19" t="s">
-        <v>19</v>
+      <c r="O20" s="27" t="s">
+        <v>88</v>
       </c>
       <c r="P20" s="19">
         <v>2030</v>
@@ -2080,10 +2089,10 @@
         <v>2050</v>
       </c>
       <c r="R20" s="19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="S20" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2096,12 +2105,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2251,15 +2257,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2283,17 +2300,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add additional SOCP constraints. Clean up Constraint logic
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kelvin Walenta\LEGO-Pyomo\data\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A756A1-3040-444B-9EB9-FC51E6791626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160D7EDC-8259-4DE8-AA1F-5A5F77B359A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5110" yWindow="2290" windowWidth="28800" windowHeight="15430" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8820" yWindow="5475" windowWidth="51810" windowHeight="20880" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="110" r:id="rId1"/>
@@ -435,7 +435,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
@@ -531,12 +531,6 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FFCE9178"/>
-      <name val="Consolas"/>
-      <family val="3"/>
     </font>
   </fonts>
   <fills count="11">
@@ -636,7 +630,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -705,9 +699,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1045,46 +1036,46 @@
       <selection activeCell="R6" sqref="R6:S6"/>
       <selection pane="topRight" activeCell="R6" sqref="R6:S6"/>
       <selection pane="bottomLeft" activeCell="R6" sqref="R6:S6"/>
-      <selection pane="bottomRight" activeCell="O8" sqref="O8:O20"/>
+      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.09765625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.8984375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="15" style="3" customWidth="1"/>
-    <col min="3" max="5" width="14.59765625" style="4" customWidth="1"/>
-    <col min="6" max="11" width="12.8984375" style="3" customWidth="1"/>
+    <col min="3" max="5" width="14.5703125" style="4" customWidth="1"/>
+    <col min="6" max="11" width="12.85546875" style="3" customWidth="1"/>
     <col min="12" max="13" width="15" style="3" customWidth="1"/>
-    <col min="14" max="14" width="28.8984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.296875" style="3" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.28515625" style="3" customWidth="1"/>
     <col min="16" max="17" width="21" style="3" customWidth="1"/>
-    <col min="18" max="19" width="25.8984375" style="3" customWidth="1"/>
+    <col min="18" max="19" width="25.85546875" style="3" customWidth="1"/>
     <col min="20" max="20" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.8984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.3984375" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.59765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="209" width="9.09765625" style="3"/>
-    <col min="210" max="210" width="9.59765625" style="3" customWidth="1"/>
-    <col min="211" max="211" width="1.59765625" style="3" customWidth="1"/>
-    <col min="212" max="212" width="9.09765625" style="3"/>
-    <col min="213" max="213" width="1.59765625" style="3" customWidth="1"/>
-    <col min="214" max="214" width="8.59765625" style="3" customWidth="1"/>
-    <col min="215" max="220" width="9.09765625" style="3"/>
-    <col min="221" max="221" width="1.59765625" style="3" customWidth="1"/>
-    <col min="222" max="225" width="9.09765625" style="3"/>
-    <col min="226" max="226" width="27.59765625" style="3" customWidth="1"/>
-    <col min="227" max="16384" width="9.09765625" style="3"/>
+    <col min="23" max="23" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="209" width="9.140625" style="3"/>
+    <col min="210" max="210" width="9.5703125" style="3" customWidth="1"/>
+    <col min="211" max="211" width="1.5703125" style="3" customWidth="1"/>
+    <col min="212" max="212" width="9.140625" style="3"/>
+    <col min="213" max="213" width="1.5703125" style="3" customWidth="1"/>
+    <col min="214" max="214" width="8.5703125" style="3" customWidth="1"/>
+    <col min="215" max="220" width="9.140625" style="3"/>
+    <col min="221" max="221" width="1.5703125" style="3" customWidth="1"/>
+    <col min="222" max="225" width="9.140625" style="3"/>
+    <col min="226" max="226" width="27.5703125" style="3" customWidth="1"/>
+    <col min="227" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B1" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B2" s="9" t="s">
         <v>21</v>
       </c>
@@ -1094,7 +1085,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>74</v>
       </c>
@@ -1153,7 +1144,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>85</v>
       </c>
@@ -1212,7 +1203,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="17"/>
       <c r="B5" s="15" t="s">
         <v>31</v>
@@ -1269,7 +1260,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="17"/>
       <c r="B6" s="16" t="s">
         <v>33</v>
@@ -1326,7 +1317,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
         <v>36</v>
@@ -1383,7 +1374,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="24"/>
       <c r="B8" s="20"/>
       <c r="C8" s="21" t="s">
@@ -1420,7 +1411,7 @@
       <c r="N8" s="25">
         <v>10</v>
       </c>
-      <c r="O8" s="27" t="s">
+      <c r="O8" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P8" s="19">
@@ -1439,7 +1430,7 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="24"/>
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
@@ -1474,7 +1465,7 @@
       </c>
       <c r="M9" s="25"/>
       <c r="N9" s="25"/>
-      <c r="O9" s="27" t="s">
+      <c r="O9" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P9" s="19">
@@ -1493,7 +1484,7 @@
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="24"/>
       <c r="B10" s="20"/>
       <c r="C10" s="21" t="s">
@@ -1528,7 +1519,7 @@
       </c>
       <c r="M10" s="25"/>
       <c r="N10" s="25"/>
-      <c r="O10" s="27" t="s">
+      <c r="O10" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P10" s="19">
@@ -1547,7 +1538,7 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A11" s="24"/>
       <c r="B11" s="20"/>
       <c r="C11" s="21" t="s">
@@ -1582,7 +1573,7 @@
       </c>
       <c r="M11" s="25"/>
       <c r="N11" s="25"/>
-      <c r="O11" s="27" t="s">
+      <c r="O11" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P11" s="19">
@@ -1601,7 +1592,7 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="24"/>
       <c r="B12" s="20"/>
       <c r="C12" s="21" t="s">
@@ -1636,7 +1627,7 @@
       </c>
       <c r="M12" s="25"/>
       <c r="N12" s="25"/>
-      <c r="O12" s="27" t="s">
+      <c r="O12" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P12" s="19">
@@ -1655,7 +1646,7 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="24"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21" t="s">
@@ -1692,7 +1683,7 @@
       <c r="N13" s="25">
         <v>100</v>
       </c>
-      <c r="O13" s="27" t="s">
+      <c r="O13" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P13" s="19">
@@ -1711,7 +1702,7 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A14" s="24"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21" t="s">
@@ -1746,7 +1737,7 @@
       </c>
       <c r="M14" s="25"/>
       <c r="N14" s="25"/>
-      <c r="O14" s="27" t="s">
+      <c r="O14" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P14" s="19">
@@ -1765,7 +1756,7 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>83</v>
       </c>
@@ -1804,7 +1795,7 @@
       <c r="N15" s="25">
         <v>90</v>
       </c>
-      <c r="O15" s="27" t="s">
+      <c r="O15" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P15" s="19">
@@ -1823,7 +1814,7 @@
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="20"/>
       <c r="C16" s="21" t="s">
@@ -1858,7 +1849,7 @@
       </c>
       <c r="M16" s="25"/>
       <c r="N16" s="25"/>
-      <c r="O16" s="27" t="s">
+      <c r="O16" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P16" s="19">
@@ -1877,7 +1868,7 @@
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>83</v>
       </c>
@@ -1914,7 +1905,7 @@
       </c>
       <c r="M17" s="25"/>
       <c r="N17" s="25"/>
-      <c r="O17" s="27" t="s">
+      <c r="O17" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P17" s="19">
@@ -1933,7 +1924,7 @@
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="24" t="s">
         <v>83</v>
       </c>
@@ -1970,7 +1961,7 @@
       </c>
       <c r="M18" s="25"/>
       <c r="N18" s="25"/>
-      <c r="O18" s="27" t="s">
+      <c r="O18" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P18" s="19">
@@ -1989,7 +1980,7 @@
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>83</v>
       </c>
@@ -2026,7 +2017,7 @@
       </c>
       <c r="M19" s="25"/>
       <c r="N19" s="25"/>
-      <c r="O19" s="27" t="s">
+      <c r="O19" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P19" s="19">
@@ -2042,7 +2033,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="24"/>
       <c r="B20" s="20"/>
       <c r="C20" s="21" t="s">
@@ -2079,7 +2070,7 @@
       <c r="N20" s="25">
         <v>50</v>
       </c>
-      <c r="O20" s="27" t="s">
+      <c r="O20" s="25" t="s">
         <v>88</v>
       </c>
       <c r="P20" s="19">
@@ -2105,12 +2096,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2256,16 +2256,15 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2281,7 +2280,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2297,12 +2296,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add cplex data extraction, add filtering of 0 value variables, add variable normalisation
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160D7EDC-8259-4DE8-AA1F-5A5F77B359A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64072B09-A78A-44E0-B081-67BF88E75F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8820" yWindow="5475" windowWidth="51810" windowHeight="20880" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36210" yWindow="1650" windowWidth="28800" windowHeight="15240" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="110" r:id="rId1"/>
@@ -423,7 +423,7 @@
     <t>YearDecom</t>
   </si>
   <si>
-    <t>SOCP</t>
+    <t>DC-OPF</t>
   </si>
 </sst>
 </file>
@@ -1036,46 +1036,46 @@
       <selection activeCell="R6" sqref="R6:S6"/>
       <selection pane="topRight" activeCell="R6" sqref="R6:S6"/>
       <selection pane="bottomLeft" activeCell="R6" sqref="R6:S6"/>
-      <selection pane="bottomRight" activeCell="L31" sqref="L31"/>
+      <selection pane="bottomRight" activeCell="O8" sqref="O8:O20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="3" customWidth="1"/>
+    <col min="1" max="1" width="4.86328125" style="3" customWidth="1"/>
     <col min="2" max="2" width="15" style="3" customWidth="1"/>
-    <col min="3" max="5" width="14.5703125" style="4" customWidth="1"/>
-    <col min="6" max="11" width="12.85546875" style="3" customWidth="1"/>
+    <col min="3" max="5" width="14.59765625" style="4" customWidth="1"/>
+    <col min="6" max="11" width="12.86328125" style="3" customWidth="1"/>
     <col min="12" max="13" width="15" style="3" customWidth="1"/>
-    <col min="14" max="14" width="28.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.28515625" style="3" customWidth="1"/>
+    <col min="14" max="14" width="28.86328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.265625" style="3" customWidth="1"/>
     <col min="16" max="17" width="21" style="3" customWidth="1"/>
-    <col min="18" max="19" width="25.85546875" style="3" customWidth="1"/>
+    <col min="18" max="19" width="25.86328125" style="3" customWidth="1"/>
     <col min="20" max="20" width="8" style="3" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.86328125" style="3" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9" style="3" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="16.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="27" max="209" width="9.140625" style="3"/>
-    <col min="210" max="210" width="9.5703125" style="3" customWidth="1"/>
-    <col min="211" max="211" width="1.5703125" style="3" customWidth="1"/>
-    <col min="212" max="212" width="9.140625" style="3"/>
-    <col min="213" max="213" width="1.5703125" style="3" customWidth="1"/>
-    <col min="214" max="214" width="8.5703125" style="3" customWidth="1"/>
-    <col min="215" max="220" width="9.140625" style="3"/>
-    <col min="221" max="221" width="1.5703125" style="3" customWidth="1"/>
-    <col min="222" max="225" width="9.140625" style="3"/>
-    <col min="226" max="226" width="27.5703125" style="3" customWidth="1"/>
-    <col min="227" max="16384" width="9.140625" style="3"/>
+    <col min="23" max="23" width="12.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.3984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.59765625" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="209" width="9.1328125" style="3"/>
+    <col min="210" max="210" width="9.59765625" style="3" customWidth="1"/>
+    <col min="211" max="211" width="1.59765625" style="3" customWidth="1"/>
+    <col min="212" max="212" width="9.1328125" style="3"/>
+    <col min="213" max="213" width="1.59765625" style="3" customWidth="1"/>
+    <col min="214" max="214" width="8.59765625" style="3" customWidth="1"/>
+    <col min="215" max="220" width="9.1328125" style="3"/>
+    <col min="221" max="221" width="1.59765625" style="3" customWidth="1"/>
+    <col min="222" max="225" width="9.1328125" style="3"/>
+    <col min="226" max="226" width="27.59765625" style="3" customWidth="1"/>
+    <col min="227" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B1" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.5">
       <c r="B2" s="9" t="s">
         <v>21</v>
       </c>
@@ -1085,7 +1085,7 @@
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A3" s="2" t="s">
         <v>74</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" s="12" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A4" s="13" t="s">
         <v>85</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:22" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" s="14" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="17"/>
       <c r="B5" s="15" t="s">
         <v>31</v>
@@ -1260,7 +1260,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:22" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" s="14" customFormat="1" ht="43" x14ac:dyDescent="0.45">
       <c r="A6" s="17"/>
       <c r="B6" s="16" t="s">
         <v>33</v>
@@ -1317,7 +1317,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
         <v>36</v>
@@ -1374,7 +1374,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A8" s="24"/>
       <c r="B8" s="20"/>
       <c r="C8" s="21" t="s">
@@ -1430,7 +1430,7 @@
       <c r="U8" s="6"/>
       <c r="V8" s="6"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A9" s="24"/>
       <c r="B9" s="20"/>
       <c r="C9" s="21" t="s">
@@ -1484,7 +1484,7 @@
       <c r="U9" s="6"/>
       <c r="V9" s="6"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A10" s="24"/>
       <c r="B10" s="20"/>
       <c r="C10" s="21" t="s">
@@ -1538,7 +1538,7 @@
       <c r="U10" s="6"/>
       <c r="V10" s="6"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A11" s="24"/>
       <c r="B11" s="20"/>
       <c r="C11" s="21" t="s">
@@ -1592,7 +1592,7 @@
       <c r="U11" s="6"/>
       <c r="V11" s="6"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A12" s="24"/>
       <c r="B12" s="20"/>
       <c r="C12" s="21" t="s">
@@ -1646,7 +1646,7 @@
       <c r="U12" s="6"/>
       <c r="V12" s="6"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A13" s="24"/>
       <c r="B13" s="20"/>
       <c r="C13" s="21" t="s">
@@ -1702,7 +1702,7 @@
       <c r="U13" s="6"/>
       <c r="V13" s="6"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A14" s="24"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21" t="s">
@@ -1756,7 +1756,7 @@
       <c r="U14" s="6"/>
       <c r="V14" s="6"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A15" s="24" t="s">
         <v>83</v>
       </c>
@@ -1814,7 +1814,7 @@
       <c r="U15" s="6"/>
       <c r="V15" s="6"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A16" s="24"/>
       <c r="B16" s="20"/>
       <c r="C16" s="21" t="s">
@@ -1868,7 +1868,7 @@
       <c r="U16" s="7"/>
       <c r="V16" s="7"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A17" s="24" t="s">
         <v>83</v>
       </c>
@@ -1924,7 +1924,7 @@
       <c r="U17" s="7"/>
       <c r="V17" s="7"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A18" s="24" t="s">
         <v>83</v>
       </c>
@@ -1980,7 +1980,7 @@
       <c r="U18" s="7"/>
       <c r="V18" s="7"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A19" s="24" t="s">
         <v>83</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.5">
       <c r="A20" s="24"/>
       <c r="B20" s="20"/>
       <c r="C20" s="21" t="s">
@@ -2096,21 +2096,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004934E3CB1C58BA43BC6E229E2BF20201" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="e33ccc94e63df24f58cb47229b46e190">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="87003a75-b64f-4b22-bf19-aa30740e3d46" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0f0f7a5bb162b669de9ce8ff8278c29f" ns2:_="">
     <xsd:import namespace="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
@@ -2256,10 +2241,35 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2281,19 +2291,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{773946F7-566C-458F-95C9-79B0CCE20E87}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="87003a75-b64f-4b22-bf19-aa30740e3d46"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add obj normalization and comparison
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64072B09-A78A-44E0-B081-67BF88E75F21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54CEDDC-FD56-4B9E-A891-6DB21BEA6DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36210" yWindow="1650" windowWidth="28800" windowHeight="15240" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38530" yWindow="4100" windowWidth="28800" windowHeight="15240" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="110" r:id="rId1"/>
@@ -1036,7 +1036,7 @@
       <selection activeCell="R6" sqref="R6:S6"/>
       <selection pane="topRight" activeCell="R6" sqref="R6:S6"/>
       <selection pane="bottomLeft" activeCell="R6" sqref="R6:S6"/>
-      <selection pane="bottomRight" activeCell="O8" sqref="O8:O20"/>
+      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2242,18 +2242,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2275,6 +2275,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2288,12 +2296,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add quadratic constraint (probably bugged) and quadratic obj handeling
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54CEDDC-FD56-4B9E-A891-6DB21BEA6DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12318BF7-9B89-4579-AB34-0F9A997532B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38530" yWindow="4100" windowWidth="28800" windowHeight="15240" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34450" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="110" r:id="rId1"/>
@@ -423,7 +423,7 @@
     <t>YearDecom</t>
   </si>
   <si>
-    <t>DC-OPF</t>
+    <t>SOCP</t>
   </si>
 </sst>
 </file>
@@ -1036,7 +1036,7 @@
       <selection activeCell="R6" sqref="R6:S6"/>
       <selection pane="topRight" activeCell="R6" sqref="R6:S6"/>
       <selection pane="bottomLeft" activeCell="R6" sqref="R6:S6"/>
-      <selection pane="bottomRight" activeCell="N27" sqref="N27"/>
+      <selection pane="bottomRight" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2242,18 +2242,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2275,14 +2275,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2296,4 +2288,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed pEnableSOCP to boolean. Add SOCP module
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF18DA9B-B972-4CD7-9DBF-9E87D9F10306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BBF73A-589C-4745-AE3B-026A5B0421A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72850" yWindow="2170" windowWidth="38620" windowHeight="21100" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37320" yWindow="5140" windowWidth="28800" windowHeight="15240" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="110" r:id="rId1"/>
@@ -1036,7 +1036,7 @@
       <selection activeCell="R6" sqref="R6:S6"/>
       <selection pane="topRight" activeCell="R6" sqref="R6:S6"/>
       <selection pane="bottomLeft" activeCell="R6" sqref="R6:S6"/>
-      <selection pane="bottomRight" activeCell="I8" sqref="I8"/>
+      <selection pane="bottomRight" activeCell="O27" sqref="O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2242,18 +2242,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2275,6 +2275,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2288,12 +2296,4 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed Bool again, add excel writer again
</commit_message>
<xml_diff>
--- a/data/example/Power_Network.xlsx
+++ b/data/example/Power_Network.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\LEGO-Pyomo\data\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84BBF73A-589C-4745-AE3B-026A5B0421A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3596A07A-18C1-43A1-8904-0638FAABFEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37320" yWindow="5140" windowWidth="28800" windowHeight="15240" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="23226" windowHeight="13866" tabRatio="517" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioA" sheetId="110" r:id="rId1"/>
@@ -423,7 +423,7 @@
     <t>YearDecom</t>
   </si>
   <si>
-    <t>SOCP</t>
+    <t>DC-OPF</t>
   </si>
 </sst>
 </file>
@@ -1032,11 +1032,11 @@
   <dimension ref="A1:V20"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
       <selection activeCell="R6" sqref="R6:S6"/>
       <selection pane="topRight" activeCell="R6" sqref="R6:S6"/>
       <selection pane="bottomLeft" activeCell="R6" sqref="R6:S6"/>
-      <selection pane="bottomRight" activeCell="O27" sqref="O27"/>
+      <selection pane="bottomRight" activeCell="O24" sqref="O24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -2242,18 +2242,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2275,14 +2275,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0155F7A0-74CD-4575-8C0B-A34C113F80FE}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -2296,4 +2288,12 @@
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{13778B2C-CE05-4B32-8196-2F381FEAC95A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>